<commit_message>
2022-04-07 FS Linux table
</commit_message>
<xml_diff>
--- a/Доп_материалы/Linux_Architecture/FileSystem_root.xlsx
+++ b/Доп_материалы/Linux_Architecture/FileSystem_root.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Каталог (директорий)</t>
   </si>
@@ -111,18 +111,12 @@
     <t>временные каталоги приложений</t>
   </si>
   <si>
-    <t>файловый интерфейс ОС</t>
-  </si>
-  <si>
     <t>аналог "Program Files"</t>
   </si>
   <si>
     <t>монтирование съёмных ФС</t>
   </si>
   <si>
-    <t>загрузчик и ядро системы</t>
-  </si>
-  <si>
     <t>монтирование сетевых ФС</t>
   </si>
   <si>
@@ -139,13 +133,485 @@
   </si>
   <si>
     <t>https://docs.atlassian.com/bamboo-specs-docs/8.1.3/specs.html?java#repositories</t>
+  </si>
+  <si>
+    <t>* не могут быть примонтированы;
+* должны быть доступны ещё до загрузки ОС</t>
+  </si>
+  <si>
+    <t>* должны быть пустыми (это точки монтирования для других ФС)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">содержит бинарные файлы, которые могут использоваться </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>всеми</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> пользователями
+В соответствии со спецификацией FHS, директория /bin должна содержать исполняемые файлы.
+Многие исполняемые файлы директории /bin являются реализациями команд (= утилиты)</t>
+    </r>
+  </si>
+  <si>
+    <t>содержит бинарные файлы, предназначенные для настройки операционной системы.
+Многие из бинарных файлов для настройки системы требуют наличия привилегий пользователя root для выполнения определенных задач</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">содержит все специфичные для машины конфигурационные файлы.
+Во многих случаях имена конфиг. файлов совпадают с именами приложений или протоколов, а в качестве расширений этих файлов используется строка </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>.conf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Описание содержимого каталогов</t>
+  </si>
+  <si>
+    <t>содержатся временные файлы, созданные системой, любыми программами или пользователями. Все пользователи имеют право записи в эту директорию.
+Файлы удаляются при каждой перезагрузке.</t>
+  </si>
+  <si>
+    <t>каталог должен содержать файлы, которые часто изменяются. Размер этих файлов постоянно увеличивается.
+Здесь содержатся файлы системных журналов, различные кеши, базы данных и т.д.
+/var/log
+/var/lib
+/var/mail
+/var/spool
+/var/lock        # файлы блокировок (= файл занят и не может быть
+                     # использован другим процессом)</t>
+  </si>
+  <si>
+    <t>файловый интерфейс ОС, информация о процессах</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">подсистема, динамически создаваемая ядром.
+содержится вся информация о запущенных процессах в реальном времени.
+По сути, это псевдофайловая система, содержащая подробную информацию о каждом процессе, его PID, имя исполняемого файла, параметры запуска, доступ к оперативной памяти и т.д.
++ здесь можно найти информацию об использовании системных ресурсов:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>/proc/cpuinfo
+/proc/meminfo
+/proc/uptime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+Кроме файлов в этом каталоге есть большая структура папок linux, из которых можно узнать достаточно много информации о системе</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Все подключенные устройства = файлы в каталоге </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>/dev/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+Структура ФС Linux и содержащиеся в папке </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>/dev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> файлы инициализируются при загрузке системы, сервисом </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>udev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">.
+ Выполняется сканирование всех подключенных устройств и создание для них специальных файлов.
+Примеры устройств:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>/dev/sda,
+/dev/sr0,
+/dev/tty1,
+/dev/usbmon0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">  и т д.</t>
+    </r>
+  </si>
+  <si>
+    <t>файлы загрузчика и ядро системы</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">содержит разделяемые библиотеки, многие из которых используются бинарными файлами из директорий </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>/bin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">/sbin
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">Библиотеки имеют имена файлов с расширением </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>*.so</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> и начинаются с префикса </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>lib*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">. (например, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>libncurses.so.5.7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">/lib/modules/&lt;kernel-version&gt;  -  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>обычно из этой директории ядро Linux загружает модули</t>
+    </r>
+  </si>
+  <si>
+    <t>(=optional applications) дополнительные программы</t>
+  </si>
+  <si>
+    <t>в эту папку устанавливаются проприетарные программы, игры или драйвера.
+Это программы созданные в виде отдельных исполняемых файлов самими производителями. 
+Такие программы устанавливаются в под-каталоги /opt/ 
+все исполняемые файлы, библиотеки и файлы конфигурации находятся в одной папке.</t>
+  </si>
+  <si>
+    <t>в этот каталог можно монтировать внешние или дополнительные файловые системы</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">/boot/grub </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">   - файлы загрузчика
+Сжатый архив ядра:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>vmlinuz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+Образ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>initrd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> - начальный RAM-диск (образ/архив ФС, который загружается в память вместе с ядром).
+Именно этот </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>init</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (из архива </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>initrd)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> будет выполнен ядром первым</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,20 +656,29 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -240,9 +715,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -262,11 +737,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -549,93 +1030,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="C2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="155.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -643,8 +1147,9 @@
         <v>26</v>
       </c>
       <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -652,8 +1157,11 @@
         <v>27</v>
       </c>
       <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
@@ -661,8 +1169,11 @@
         <v>28</v>
       </c>
       <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -670,107 +1181,131 @@
         <v>29</v>
       </c>
       <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="203.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="8" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="C15:C16"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B21" r:id="rId1"/>
     <hyperlink ref="B23" r:id="rId2"/>
     <hyperlink ref="B25" r:id="rId3" location="repositories"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2022-04-13 Finisher table 'Filesystem_Linux'. Continued article 'Bash'
</commit_message>
<xml_diff>
--- a/Доп_материалы/Linux_Architecture/FileSystem_root.xlsx
+++ b/Доп_материалы/Linux_Architecture/FileSystem_root.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Краткое описание хранящихся файлов</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>монтирование сетевых ФС</t>
-  </si>
-  <si>
-    <t>размещение Web-сайтов, FTP,…</t>
   </si>
   <si>
     <t>содержит бинарные файлы, предназначенные для настройки операционной системы.
@@ -123,16 +120,6 @@
   <si>
     <t>содержатся временные файлы, созданные системой, любыми программами или пользователями. Все пользователи имеют право записи в эту директорию.
 Файлы удаляются при каждой перезагрузке.</t>
-  </si>
-  <si>
-    <t>каталог должен содержать файлы, которые часто изменяются. Размер этих файлов постоянно увеличивается.
-Здесь содержатся файлы системных журналов, различные кеши, базы данных и т.д.
-/var/log
-/var/lib
-/var/mail
-/var/spool
-/var/lock        # файлы блокировок (= файл занят и не может быть
-                     # использован другим процессом)</t>
   </si>
   <si>
     <t>файловый интерфейс ОС, информация о процессах</t>
@@ -477,232 +464,6 @@
 В некоторых системах /tmp размещается на маленьком разделе диска, в этом случае /var/tmp - это каталог в котором можно размещать большие временные файлы</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Здесь находятся исполняемые файлы, исходники программ, различные ресурсы приложений, картинки, музыка и документация.
-Подкаталоги:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/bin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – содержит большую часть утилит, используемых пользователем;
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/include</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – файлы заголовков, включаемых в С-программы;
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/lib</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – библиотеки;
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/local</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – локальная иерархия;
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/sbin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – содержит не жизненно необходимые системные исполняемые файлы;
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/share</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – архитектурно-независимые данные (документация, шрифты, программы на скриптовых языках и другие неизменяемые данные, которые могут быть использованы через сетевую файловую систему с любой версией программ и для любой архитектуры процессора);
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/X11R6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – X Window System, версия 11, выпуск 6;
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/games</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – игры и образовательные программы;
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/src</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – исходные коды.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>/usr/bin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve"> – пользовательские программы</t>
-    </r>
-  </si>
-  <si>
     <t>«домашний» каталог администратора (пользователя root = суперпользователя)</t>
   </si>
   <si>
@@ -906,13 +667,342 @@
   </si>
   <si>
     <t>файлы конфигураций</t>
+  </si>
+  <si>
+    <t>данные сервисных служб</t>
+  </si>
+  <si>
+    <t>присуствует не во всех дистрибутивах; содержит "данные для сервисов, предоставляемых системой (напр., Apache хранит данные сайта пользователя)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">каталог должен содержать файлы, которые часто изменяются. Размер этих файлов постоянно увеличивается.
+Здесь содержатся файлы системных журналов, различные кеши, базы данных и т.д.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/var/log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">        # большинство файлов логов всех программ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/var/lib</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">        # файлы базы данных 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/var/mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">      #  все полученные | отправленные электронные письма
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">/var/spool </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">  # очереди печати на принтере/работа набора программ cups
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/var/lock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">      # файлы блокировок (= файл занят и не может быть
+                        # использован другим процессом)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Здесь находятся исполняемые файлы, исходники программ, различные ресурсы приложений, картинки, музыка и документация.
+Подкаталоги:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/bin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – содержит большую часть утилит, используемых пользователем;
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/include</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – файлы заголовков, включаемых в С-программы;
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/lib</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – библиотеки;
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/local</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – локальная иерархия;
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/sbin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – содержит не жизненно необходимые системные исполняемые файлы;
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/share</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – архитектурно-независимые данные (документация, шрифты, программы на скриптовых языках и другие неизменяемые данные, которые могут быть использованы через сетевую файловую систему с любой версией программ и для любой архитектуры процессора);
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/X11R6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – X Window System, версия 11, выпуск 6;
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – игры и образовательные программы;
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/src</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – исходные коды.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Courier"/>
+        <family val="3"/>
+      </rPr>
+      <t>/usr/bin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> – пользовательские программы</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -991,13 +1081,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1010,6 +1093,18 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1109,7 +1204,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1404,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1419,13 +1514,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="13"/>
     </row>
@@ -1437,10 +1532,10 @@
         <v>19</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.25">
@@ -1452,7 +1547,7 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
@@ -1464,7 +1559,7 @@
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
@@ -1472,11 +1567,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
@@ -1488,7 +1583,7 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1500,7 +1595,7 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1512,7 +1607,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="242.25" x14ac:dyDescent="0.25">
@@ -1520,13 +1615,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
@@ -1538,7 +1633,7 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -1550,7 +1645,7 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="63" x14ac:dyDescent="0.25">
@@ -1562,7 +1657,7 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="171.75" x14ac:dyDescent="0.25">
@@ -1570,11 +1665,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
@@ -1582,13 +1677,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1599,10 +1694,10 @@
         <v>28</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1610,11 +1705,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
@@ -1622,11 +1717,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -1634,22 +1729,24 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>

</xml_diff>